<commit_message>
Update: working envelope generator & test application (Synth)
</commit_message>
<xml_diff>
--- a/Documentation/AmiGUS/AmiGUS_Register_Map.xlsx
+++ b/Documentation/AmiGUS/AmiGUS_Register_Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achte\OneDrive\Dokumente\GitHub\AmiGUS\AmiGUS-pub\Documentation\AmiGUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A03E7CF-F749-4C37-B78D-5F84935B1D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44D9257-1D33-4493-8287-27BA29739479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15320" xr2:uid="{25B183AC-6DDA-4ECE-8C4C-D106BCA74C97}"/>
+    <workbookView xWindow="40180" yWindow="690" windowWidth="12920" windowHeight="18910" activeTab="2" xr2:uid="{25B183AC-6DDA-4ECE-8C4C-D106BCA74C97}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Register" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="480">
   <si>
     <t>Address Offset</t>
   </si>
@@ -1478,6 +1478,12 @@
   </si>
   <si>
     <t>1000 = 64000 Hz</t>
+  </si>
+  <si>
+    <t>Voice N Envelope RESET</t>
+  </si>
+  <si>
+    <t>Reset envelope generator</t>
   </si>
 </sst>
 </file>
@@ -2167,7 +2173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2528,10 +2534,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2882,21 +2893,21 @@
   </sheetPr>
   <dimension ref="A1:H150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="I136" sqref="I136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="31.7265625" customWidth="1"/>
-    <col min="4" max="4" width="4.08984375" customWidth="1"/>
-    <col min="5" max="5" width="5.26953125" customWidth="1"/>
-    <col min="6" max="6" width="29.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.23046875" customWidth="1"/>
+    <col min="3" max="3" width="31.69140625" customWidth="1"/>
+    <col min="4" max="4" width="4.07421875" customWidth="1"/>
+    <col min="5" max="5" width="5.23046875" customWidth="1"/>
+    <col min="6" max="6" width="29.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="64"/>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -2906,19 +2917,19 @@
       <c r="G1" s="64"/>
       <c r="H1" s="64"/>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="64"/>
-      <c r="B2" s="189" t="s">
+      <c r="B2" s="192" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="190"/>
-      <c r="F2" s="191"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="194"/>
       <c r="G2" s="64"/>
       <c r="H2" s="64"/>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="64"/>
       <c r="B3" s="83" t="s">
         <v>0</v>
@@ -2938,7 +2949,7 @@
       <c r="G3" s="64"/>
       <c r="H3" s="64"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="64"/>
       <c r="B4" s="156" t="s">
         <v>4</v>
@@ -2958,7 +2969,7 @@
       <c r="G4" s="64"/>
       <c r="H4" s="64"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="64"/>
       <c r="B5" s="156"/>
       <c r="C5" s="125"/>
@@ -2974,7 +2985,7 @@
       <c r="G5" s="64"/>
       <c r="H5" s="64"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="64"/>
       <c r="B6" s="156"/>
       <c r="C6" s="125"/>
@@ -2990,7 +3001,7 @@
       <c r="G6" s="64"/>
       <c r="H6" s="64"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="64"/>
       <c r="B7" s="156"/>
       <c r="C7" s="97"/>
@@ -3006,7 +3017,7 @@
       <c r="G7" s="64"/>
       <c r="H7" s="64"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="64"/>
       <c r="B8" s="156"/>
       <c r="C8" s="125"/>
@@ -3022,7 +3033,7 @@
       <c r="G8" s="64"/>
       <c r="H8" s="64"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="64"/>
       <c r="B9" s="156"/>
       <c r="C9" s="125"/>
@@ -3038,7 +3049,7 @@
       <c r="G9" s="64"/>
       <c r="H9" s="64"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="64"/>
       <c r="B10" s="156"/>
       <c r="C10" s="125"/>
@@ -3054,7 +3065,7 @@
       <c r="G10" s="64"/>
       <c r="H10" s="64"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="64"/>
       <c r="B11" s="156"/>
       <c r="C11" s="125"/>
@@ -3070,7 +3081,7 @@
       <c r="G11" s="64"/>
       <c r="H11" s="64"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="64"/>
       <c r="B12" s="156"/>
       <c r="C12" s="125"/>
@@ -3086,7 +3097,7 @@
       <c r="G12" s="64"/>
       <c r="H12" s="64"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="64"/>
       <c r="B13" s="156"/>
       <c r="C13" s="125"/>
@@ -3098,7 +3109,7 @@
       <c r="G13" s="64"/>
       <c r="H13" s="64"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="64"/>
       <c r="B14" s="157" t="s">
         <v>16</v>
@@ -3118,7 +3129,7 @@
       <c r="G14" s="64"/>
       <c r="H14" s="64"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="64"/>
       <c r="B15" s="156"/>
       <c r="C15" s="125"/>
@@ -3134,7 +3145,7 @@
       <c r="G15" s="64"/>
       <c r="H15" s="64"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="64"/>
       <c r="B16" s="156"/>
       <c r="C16" s="125"/>
@@ -3150,7 +3161,7 @@
       <c r="G16" s="64"/>
       <c r="H16" s="64"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="64"/>
       <c r="B17" s="156"/>
       <c r="C17" s="125"/>
@@ -3166,7 +3177,7 @@
       <c r="G17" s="64"/>
       <c r="H17" s="64"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="64"/>
       <c r="B18" s="156"/>
       <c r="C18" s="125"/>
@@ -3182,7 +3193,7 @@
       <c r="G18" s="64"/>
       <c r="H18" s="64"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="64"/>
       <c r="B19" s="156"/>
       <c r="C19" s="125"/>
@@ -3198,7 +3209,7 @@
       <c r="G19" s="64"/>
       <c r="H19" s="64"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" s="64"/>
       <c r="B20" s="156"/>
       <c r="C20" s="125"/>
@@ -3214,7 +3225,7 @@
       <c r="G20" s="64"/>
       <c r="H20" s="64"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="64"/>
       <c r="B21" s="156"/>
       <c r="C21" s="125"/>
@@ -3230,7 +3241,7 @@
       <c r="G21" s="64"/>
       <c r="H21" s="64"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" s="64"/>
       <c r="B22" s="156"/>
       <c r="C22" s="125"/>
@@ -3246,7 +3257,7 @@
       <c r="G22" s="64"/>
       <c r="H22" s="64"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="64"/>
       <c r="B23" s="158"/>
       <c r="C23" s="99"/>
@@ -3258,7 +3269,7 @@
       <c r="G23" s="64"/>
       <c r="H23" s="64"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="64"/>
       <c r="B24" s="157" t="s">
         <v>17</v>
@@ -3278,7 +3289,7 @@
       <c r="G24" s="64"/>
       <c r="H24" s="64"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" s="64"/>
       <c r="B25" s="156"/>
       <c r="C25" s="125"/>
@@ -3290,7 +3301,7 @@
       <c r="G25" s="64"/>
       <c r="H25" s="64"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" s="64"/>
       <c r="B26" s="156"/>
       <c r="C26" s="125"/>
@@ -3302,7 +3313,7 @@
       <c r="G26" s="64"/>
       <c r="H26" s="64"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" s="64"/>
       <c r="B27" s="156"/>
       <c r="C27" s="125"/>
@@ -3314,7 +3325,7 @@
       <c r="G27" s="64"/>
       <c r="H27" s="64"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28" s="64"/>
       <c r="B28" s="156"/>
       <c r="C28" s="125"/>
@@ -3326,7 +3337,7 @@
       <c r="G28" s="64"/>
       <c r="H28" s="64"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" s="64"/>
       <c r="B29" s="156"/>
       <c r="C29" s="125"/>
@@ -3338,7 +3349,7 @@
       <c r="G29" s="64"/>
       <c r="H29" s="64"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" s="64"/>
       <c r="B30" s="156"/>
       <c r="C30" s="97"/>
@@ -3354,7 +3365,7 @@
       <c r="G30" s="64"/>
       <c r="H30" s="64"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="64"/>
       <c r="B31" s="156"/>
       <c r="C31" s="125"/>
@@ -3369,7 +3380,7 @@
       </c>
       <c r="H31" s="64"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32" s="64"/>
       <c r="B32" s="156"/>
       <c r="C32" s="125"/>
@@ -3380,7 +3391,7 @@
       </c>
       <c r="H32" s="64"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33" s="64"/>
       <c r="B33" s="156"/>
       <c r="C33" s="125"/>
@@ -3395,7 +3406,7 @@
       </c>
       <c r="H33" s="64"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A34" s="64"/>
       <c r="B34" s="156"/>
       <c r="C34" s="125"/>
@@ -3406,7 +3417,7 @@
       </c>
       <c r="H34" s="64"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A35" s="64"/>
       <c r="B35" s="157" t="s">
         <v>18</v>
@@ -3426,7 +3437,7 @@
       <c r="G35" s="64"/>
       <c r="H35" s="64"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" s="64"/>
       <c r="B36" s="156"/>
       <c r="C36" s="125"/>
@@ -3438,7 +3449,7 @@
       <c r="G36" s="64"/>
       <c r="H36" s="64"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" s="64"/>
       <c r="B37" s="156"/>
       <c r="C37" s="125"/>
@@ -3450,7 +3461,7 @@
       <c r="G37" s="64"/>
       <c r="H37" s="64"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="64"/>
       <c r="B38" s="156"/>
       <c r="C38" s="125"/>
@@ -3462,7 +3473,7 @@
       <c r="G38" s="64"/>
       <c r="H38" s="64"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A39" s="64"/>
       <c r="B39" s="156"/>
       <c r="C39" s="125"/>
@@ -3474,7 +3485,7 @@
       <c r="G39" s="64"/>
       <c r="H39" s="64"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A40" s="64"/>
       <c r="B40" s="156"/>
       <c r="C40" s="125"/>
@@ -3486,7 +3497,7 @@
       <c r="G40" s="64"/>
       <c r="H40" s="64"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A41" s="64"/>
       <c r="B41" s="156"/>
       <c r="C41" s="125"/>
@@ -3498,7 +3509,7 @@
       <c r="G41" s="64"/>
       <c r="H41" s="64"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A42" s="64"/>
       <c r="B42" s="156"/>
       <c r="C42" s="125"/>
@@ -3510,7 +3521,7 @@
       <c r="G42" s="64"/>
       <c r="H42" s="64"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A43" s="64"/>
       <c r="B43" s="156"/>
       <c r="C43" s="125"/>
@@ -3522,7 +3533,7 @@
       <c r="G43" s="64"/>
       <c r="H43" s="64"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A44" s="64"/>
       <c r="B44" s="156"/>
       <c r="C44" s="125"/>
@@ -3538,7 +3549,7 @@
       <c r="G44" s="64"/>
       <c r="H44" s="64"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A45" s="64"/>
       <c r="B45" s="156"/>
       <c r="C45" s="125"/>
@@ -3550,7 +3561,7 @@
       <c r="G45" s="64"/>
       <c r="H45" s="64"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A46" s="64"/>
       <c r="B46" s="156"/>
       <c r="C46" s="125"/>
@@ -3566,7 +3577,7 @@
       <c r="G46" s="64"/>
       <c r="H46" s="64"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A47" s="64"/>
       <c r="B47" s="158"/>
       <c r="C47" s="99"/>
@@ -3578,7 +3589,7 @@
       <c r="G47" s="64"/>
       <c r="H47" s="64"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A48" s="64"/>
       <c r="B48" s="159" t="s">
         <v>21</v>
@@ -3598,7 +3609,7 @@
       <c r="G48" s="64"/>
       <c r="H48" s="64"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A49" s="64"/>
       <c r="B49" s="159" t="s">
         <v>24</v>
@@ -3618,7 +3629,7 @@
       <c r="G49" s="64"/>
       <c r="H49" s="64"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A50" s="64"/>
       <c r="B50" s="159" t="s">
         <v>30</v>
@@ -3638,7 +3649,7 @@
       <c r="G50" s="64"/>
       <c r="H50" s="64"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A51" s="64"/>
       <c r="B51" s="159" t="s">
         <v>31</v>
@@ -3658,7 +3669,7 @@
       <c r="G51" s="64"/>
       <c r="H51" s="64"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A52" s="64"/>
       <c r="B52" s="159" t="s">
         <v>182</v>
@@ -3678,7 +3689,7 @@
       <c r="G52" s="64"/>
       <c r="H52" s="64"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A53" s="64"/>
       <c r="B53" s="159" t="s">
         <v>188</v>
@@ -3698,7 +3709,7 @@
       <c r="G53" s="64"/>
       <c r="H53" s="64"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A54" s="64"/>
       <c r="B54" s="91" t="s">
         <v>37</v>
@@ -3718,7 +3729,7 @@
       <c r="G54" s="64"/>
       <c r="H54" s="64"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A55" s="64"/>
       <c r="B55" s="91" t="s">
         <v>40</v>
@@ -3738,7 +3749,7 @@
       <c r="G55" s="64"/>
       <c r="H55" s="64"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A56" s="64"/>
       <c r="B56" s="91" t="s">
         <v>43</v>
@@ -3758,7 +3769,7 @@
       <c r="G56" s="64"/>
       <c r="H56" s="64"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A57" s="64"/>
       <c r="B57" s="91" t="s">
         <v>51</v>
@@ -3778,7 +3789,7 @@
       <c r="G57" s="64"/>
       <c r="H57" s="64"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A58" s="64"/>
       <c r="B58" s="91" t="s">
         <v>50</v>
@@ -3798,7 +3809,7 @@
       <c r="G58" s="64"/>
       <c r="H58" s="64"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A59" s="64"/>
       <c r="B59" s="89" t="s">
         <v>77</v>
@@ -3818,7 +3829,7 @@
       <c r="G59" s="64"/>
       <c r="H59" s="64"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A60" s="64"/>
       <c r="B60" s="90"/>
       <c r="C60" s="103"/>
@@ -3830,7 +3841,7 @@
       <c r="G60" s="64"/>
       <c r="H60" s="64"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A61" s="64"/>
       <c r="B61" s="159" t="s">
         <v>56</v>
@@ -3850,7 +3861,7 @@
       <c r="G61" s="64"/>
       <c r="H61" s="64"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A62" s="64"/>
       <c r="B62" s="159" t="s">
         <v>57</v>
@@ -3870,7 +3881,7 @@
       <c r="G62" s="64"/>
       <c r="H62" s="64"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A63" s="64"/>
       <c r="B63" s="159" t="s">
         <v>58</v>
@@ -3890,7 +3901,7 @@
       <c r="G63" s="64"/>
       <c r="H63" s="64"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A64" s="64"/>
       <c r="B64" s="159" t="s">
         <v>59</v>
@@ -3910,7 +3921,7 @@
       <c r="G64" s="64"/>
       <c r="H64" s="64"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A65" s="64"/>
       <c r="B65" s="159" t="s">
         <v>60</v>
@@ -3930,7 +3941,7 @@
       <c r="G65" s="64"/>
       <c r="H65" s="64"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A66" s="64"/>
       <c r="B66" s="159" t="s">
         <v>65</v>
@@ -3950,7 +3961,7 @@
       <c r="G66" s="64"/>
       <c r="H66" s="64"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A67" s="64"/>
       <c r="B67" s="159" t="s">
         <v>66</v>
@@ -3970,7 +3981,7 @@
       <c r="G67" s="64"/>
       <c r="H67" s="64"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A68" s="64"/>
       <c r="B68" s="159" t="s">
         <v>67</v>
@@ -3990,7 +4001,7 @@
       <c r="G68" s="64"/>
       <c r="H68" s="64"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A69" s="64"/>
       <c r="B69" s="159" t="s">
         <v>61</v>
@@ -4010,7 +4021,7 @@
       <c r="G69" s="64"/>
       <c r="H69" s="64"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A70" s="64"/>
       <c r="B70" s="159" t="s">
         <v>62</v>
@@ -4030,7 +4041,7 @@
       <c r="G70" s="64"/>
       <c r="H70" s="64"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A71" s="64"/>
       <c r="B71" s="159" t="s">
         <v>63</v>
@@ -4050,7 +4061,7 @@
       <c r="G71" s="64"/>
       <c r="H71" s="64"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A72" s="64"/>
       <c r="B72" s="159" t="s">
         <v>64</v>
@@ -4070,7 +4081,7 @@
       <c r="G72" s="64"/>
       <c r="H72" s="64"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A73" s="64"/>
       <c r="B73" s="157" t="s">
         <v>417</v>
@@ -4090,7 +4101,7 @@
       <c r="G73" s="64"/>
       <c r="H73" s="64"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A74" s="64"/>
       <c r="B74" s="156"/>
       <c r="C74" s="97"/>
@@ -4102,7 +4113,7 @@
       <c r="G74" s="64"/>
       <c r="H74" s="64"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A75" s="64"/>
       <c r="B75" s="156"/>
       <c r="C75" s="97"/>
@@ -4116,7 +4127,7 @@
       <c r="G75" s="64"/>
       <c r="H75" s="64"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A76" s="64"/>
       <c r="B76" s="160"/>
       <c r="C76" s="97"/>
@@ -4128,7 +4139,7 @@
       <c r="G76" s="64"/>
       <c r="H76" s="64"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A77" s="64"/>
       <c r="B77" s="161" t="s">
         <v>419</v>
@@ -4148,7 +4159,7 @@
       <c r="G77" s="64"/>
       <c r="H77" s="64"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A78" s="64"/>
       <c r="B78" s="161" t="s">
         <v>421</v>
@@ -4168,7 +4179,7 @@
       <c r="G78" s="64"/>
       <c r="H78" s="64"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A79" s="64"/>
       <c r="B79" s="161" t="s">
         <v>424</v>
@@ -4188,7 +4199,7 @@
       <c r="G79" s="64"/>
       <c r="H79" s="64"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A80" s="64"/>
       <c r="B80" s="92" t="s">
         <v>362</v>
@@ -4206,7 +4217,7 @@
       <c r="G80" s="64"/>
       <c r="H80" s="64"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A81" s="64"/>
       <c r="B81" s="92" t="s">
         <v>368</v>
@@ -4224,7 +4235,7 @@
       <c r="G81" s="64"/>
       <c r="H81" s="64"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A82" s="64"/>
       <c r="B82" s="92" t="s">
         <v>369</v>
@@ -4242,7 +4253,7 @@
       <c r="G82" s="64"/>
       <c r="H82" s="64"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A83" s="64"/>
       <c r="B83" s="92" t="s">
         <v>370</v>
@@ -4260,7 +4271,7 @@
       <c r="G83" s="64"/>
       <c r="H83" s="64"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A84" s="64"/>
       <c r="B84" s="92" t="s">
         <v>377</v>
@@ -4278,7 +4289,7 @@
       <c r="G84" s="64"/>
       <c r="H84" s="64"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A85" s="64"/>
       <c r="B85" s="92" t="s">
         <v>378</v>
@@ -4296,7 +4307,7 @@
       <c r="G85" s="64"/>
       <c r="H85" s="64"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A86" s="64"/>
       <c r="B86" s="92" t="s">
         <v>379</v>
@@ -4314,7 +4325,7 @@
       <c r="G86" s="64"/>
       <c r="H86" s="64"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A87" s="64"/>
       <c r="B87" s="92" t="s">
         <v>380</v>
@@ -4332,7 +4343,7 @@
       <c r="G87" s="64"/>
       <c r="H87" s="64"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A88" s="64"/>
       <c r="B88" s="92" t="s">
         <v>381</v>
@@ -4350,7 +4361,7 @@
       <c r="G88" s="64"/>
       <c r="H88" s="64"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A89" s="64"/>
       <c r="B89" s="92" t="s">
         <v>382</v>
@@ -4368,7 +4379,7 @@
       <c r="G89" s="64"/>
       <c r="H89" s="64"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A90" s="64"/>
       <c r="B90" s="91" t="s">
         <v>383</v>
@@ -4386,7 +4397,7 @@
       <c r="G90" s="64"/>
       <c r="H90" s="64"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A91" s="64"/>
       <c r="B91" s="93" t="s">
         <v>384</v>
@@ -4406,7 +4417,7 @@
       <c r="G91" s="64"/>
       <c r="H91" s="64"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A92" s="64"/>
       <c r="B92" s="90"/>
       <c r="C92" s="103"/>
@@ -4418,7 +4429,7 @@
       <c r="G92" s="64"/>
       <c r="H92" s="64"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A93" s="64"/>
       <c r="B93" s="160" t="s">
         <v>465</v>
@@ -4438,7 +4449,7 @@
       <c r="G93" s="64"/>
       <c r="H93" s="64"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A94" s="64"/>
       <c r="B94" s="160"/>
       <c r="C94" s="97"/>
@@ -4450,7 +4461,7 @@
       <c r="G94" s="64"/>
       <c r="H94" s="64"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A95" s="64"/>
       <c r="B95" s="158"/>
       <c r="C95" s="97"/>
@@ -4462,7 +4473,7 @@
       <c r="G95" s="64"/>
       <c r="H95" s="64"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A96" s="64"/>
       <c r="B96" s="160" t="s">
         <v>473</v>
@@ -4482,7 +4493,7 @@
       <c r="G96" s="64"/>
       <c r="H96" s="64"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A97" s="64"/>
       <c r="B97" s="160"/>
       <c r="C97" s="97"/>
@@ -4496,7 +4507,7 @@
       <c r="G97" s="64"/>
       <c r="H97" s="64"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A98" s="64"/>
       <c r="B98" s="158"/>
       <c r="C98" s="103"/>
@@ -4508,7 +4519,7 @@
       <c r="G98" s="64"/>
       <c r="H98" s="64"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A99" s="64"/>
       <c r="B99" s="92" t="s">
         <v>275</v>
@@ -4528,7 +4539,7 @@
       <c r="G99" s="64"/>
       <c r="H99" s="64"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A100" s="64"/>
       <c r="B100" s="87"/>
       <c r="C100" s="97"/>
@@ -4540,7 +4551,7 @@
       <c r="G100" s="64"/>
       <c r="H100" s="64"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A101" s="64"/>
       <c r="B101" s="87"/>
       <c r="C101" s="97"/>
@@ -4556,7 +4567,7 @@
       <c r="G101" s="64"/>
       <c r="H101" s="64"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A102" s="64"/>
       <c r="B102" s="87"/>
       <c r="C102" s="97"/>
@@ -4568,7 +4579,7 @@
       <c r="G102" s="64"/>
       <c r="H102" s="64"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A103" s="64"/>
       <c r="B103" s="93"/>
       <c r="C103" s="97"/>
@@ -4580,7 +4591,7 @@
       <c r="G103" s="64"/>
       <c r="H103" s="64"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A104" s="64"/>
       <c r="B104" s="87"/>
       <c r="C104" s="97"/>
@@ -4592,7 +4603,7 @@
       <c r="G104" s="64"/>
       <c r="H104" s="64"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A105" s="64"/>
       <c r="B105" s="87"/>
       <c r="C105" s="97"/>
@@ -4608,7 +4619,7 @@
       <c r="G105" s="64"/>
       <c r="H105" s="64"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A106" s="64"/>
       <c r="B106" s="87"/>
       <c r="C106" s="97"/>
@@ -4620,7 +4631,7 @@
       <c r="G106" s="64"/>
       <c r="H106" s="64"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A107" s="64"/>
       <c r="B107" s="87"/>
       <c r="C107" s="97"/>
@@ -4636,7 +4647,7 @@
       <c r="G107" s="64"/>
       <c r="H107" s="64"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A108" s="64"/>
       <c r="B108" s="93"/>
       <c r="C108" s="97"/>
@@ -4648,7 +4659,7 @@
       <c r="G108" s="64"/>
       <c r="H108" s="64"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A109" s="64"/>
       <c r="B109" s="89" t="s">
         <v>284</v>
@@ -4668,7 +4679,7 @@
       <c r="G109" s="64"/>
       <c r="H109" s="64"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A110" s="64"/>
       <c r="B110" s="87"/>
       <c r="C110" s="97"/>
@@ -4680,7 +4691,7 @@
       <c r="G110" s="64"/>
       <c r="H110" s="64"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A111" s="64"/>
       <c r="B111" s="93"/>
       <c r="C111" s="97"/>
@@ -4692,7 +4703,7 @@
       <c r="G111" s="64"/>
       <c r="H111" s="64"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A112" s="64"/>
       <c r="B112" s="87"/>
       <c r="C112" s="97"/>
@@ -4704,7 +4715,7 @@
       <c r="G112" s="64"/>
       <c r="H112" s="64"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A113" s="64"/>
       <c r="B113" s="87"/>
       <c r="C113" s="97"/>
@@ -4716,7 +4727,7 @@
       <c r="G113" s="64"/>
       <c r="H113" s="64"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A114" s="64"/>
       <c r="B114" s="93"/>
       <c r="C114" s="97"/>
@@ -4728,7 +4739,7 @@
       <c r="G114" s="64"/>
       <c r="H114" s="64"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A115" s="64"/>
       <c r="B115" s="87"/>
       <c r="C115" s="97"/>
@@ -4740,7 +4751,7 @@
       <c r="G115" s="64"/>
       <c r="H115" s="64"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A116" s="64"/>
       <c r="B116" s="87"/>
       <c r="C116" s="97"/>
@@ -4752,7 +4763,7 @@
       <c r="G116" s="64"/>
       <c r="H116" s="64"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A117" s="64"/>
       <c r="B117" s="87"/>
       <c r="C117" s="97"/>
@@ -4764,7 +4775,7 @@
       <c r="G117" s="64"/>
       <c r="H117" s="64"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A118" s="64"/>
       <c r="B118" s="87"/>
       <c r="C118" s="97"/>
@@ -4776,7 +4787,7 @@
       <c r="G118" s="64"/>
       <c r="H118" s="64"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A119" s="64"/>
       <c r="B119" s="87"/>
       <c r="C119" s="97"/>
@@ -4792,7 +4803,7 @@
       <c r="G119" s="64"/>
       <c r="H119" s="64"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A120" s="64"/>
       <c r="B120" s="87"/>
       <c r="C120" s="97"/>
@@ -4804,7 +4815,7 @@
       <c r="G120" s="64"/>
       <c r="H120" s="64"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A121" s="64"/>
       <c r="B121" s="87"/>
       <c r="C121" s="97"/>
@@ -4816,7 +4827,7 @@
       <c r="G121" s="64"/>
       <c r="H121" s="64"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A122" s="64"/>
       <c r="B122" s="87"/>
       <c r="C122" s="97"/>
@@ -4828,7 +4839,7 @@
       <c r="G122" s="64"/>
       <c r="H122" s="64"/>
     </row>
-    <row r="123" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A123" s="64"/>
       <c r="B123" s="87"/>
       <c r="C123" s="97"/>
@@ -4840,7 +4851,7 @@
       <c r="G123" s="64"/>
       <c r="H123" s="64"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A124" s="64"/>
       <c r="B124" s="87"/>
       <c r="C124" s="97"/>
@@ -4856,7 +4867,7 @@
       <c r="G124" s="64"/>
       <c r="H124" s="64"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A125" s="64"/>
       <c r="B125" s="93"/>
       <c r="C125" s="97"/>
@@ -4868,7 +4879,7 @@
       <c r="G125" s="64"/>
       <c r="H125" s="64"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A126" s="64"/>
       <c r="B126" s="89" t="s">
         <v>316</v>
@@ -4888,7 +4899,7 @@
       <c r="G126" s="64"/>
       <c r="H126" s="64"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A127" s="64"/>
       <c r="B127" s="91" t="s">
         <v>317</v>
@@ -4908,7 +4919,7 @@
       <c r="G127" s="64"/>
       <c r="H127" s="64"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A128" s="64"/>
       <c r="B128" s="91" t="s">
         <v>318</v>
@@ -4928,7 +4939,7 @@
       <c r="G128" s="64"/>
       <c r="H128" s="64"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A129" s="64"/>
       <c r="B129" s="91" t="s">
         <v>319</v>
@@ -4948,7 +4959,7 @@
       <c r="G129" s="64"/>
       <c r="H129" s="64"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A130" s="64"/>
       <c r="B130" s="91" t="s">
         <v>320</v>
@@ -4968,7 +4979,7 @@
       <c r="G130" s="64"/>
       <c r="H130" s="64"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A131" s="64"/>
       <c r="B131" s="91" t="s">
         <v>321</v>
@@ -4988,7 +4999,7 @@
       <c r="G131" s="64"/>
       <c r="H131" s="64"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A132" s="64"/>
       <c r="B132" s="161" t="s">
         <v>68</v>
@@ -5008,7 +5019,7 @@
       <c r="G132" s="64"/>
       <c r="H132" s="64"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A133" s="64"/>
       <c r="B133" s="160"/>
       <c r="C133" s="97"/>
@@ -5020,7 +5031,7 @@
       <c r="G133" s="64"/>
       <c r="H133" s="64"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A134" s="64"/>
       <c r="B134" s="160"/>
       <c r="C134" s="97"/>
@@ -5036,9 +5047,9 @@
       <c r="G134" s="64"/>
       <c r="H134" s="64"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A135" s="64"/>
-      <c r="B135" s="187"/>
+      <c r="B135" s="186"/>
       <c r="C135" s="103"/>
       <c r="D135" s="59"/>
       <c r="E135" s="39"/>
@@ -5048,7 +5059,7 @@
       <c r="G135" s="64"/>
       <c r="H135" s="64"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A136" s="64"/>
       <c r="B136" s="161" t="s">
         <v>74</v>
@@ -5068,9 +5079,9 @@
       <c r="G136" s="64"/>
       <c r="H136" s="64"/>
     </row>
-    <row r="137" spans="1:8" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" ht="23.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A137" s="64"/>
-      <c r="B137" s="188" t="s">
+      <c r="B137" s="187" t="s">
         <v>444</v>
       </c>
       <c r="C137" s="165" t="s">
@@ -5088,7 +5099,7 @@
       <c r="G137" s="64"/>
       <c r="H137" s="64"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A138" s="64"/>
       <c r="B138" s="87" t="s">
         <v>343</v>
@@ -5108,7 +5119,7 @@
       <c r="G138" s="64"/>
       <c r="H138" s="64"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A139" s="64"/>
       <c r="B139" s="93"/>
       <c r="C139" s="131"/>
@@ -5120,7 +5131,7 @@
       <c r="G139" s="64"/>
       <c r="H139" s="64"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A140" s="64"/>
       <c r="B140" s="93"/>
       <c r="C140" s="56"/>
@@ -5136,7 +5147,7 @@
       <c r="G140" s="64"/>
       <c r="H140" s="64"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A141" s="64"/>
       <c r="B141" s="93"/>
       <c r="C141" s="133"/>
@@ -5148,7 +5159,7 @@
       <c r="G141" s="64"/>
       <c r="H141" s="64"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A142" s="64"/>
       <c r="B142" s="92" t="s">
         <v>349</v>
@@ -5168,7 +5179,7 @@
       <c r="G142" s="64"/>
       <c r="H142" s="64"/>
     </row>
-    <row r="143" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A143" s="64"/>
       <c r="B143" s="94" t="s">
         <v>353</v>
@@ -5188,7 +5199,7 @@
       <c r="G143" s="64"/>
       <c r="H143" s="64"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A144" s="64"/>
       <c r="B144" s="88"/>
       <c r="C144" s="88"/>
@@ -5198,7 +5209,7 @@
       <c r="G144" s="64"/>
       <c r="H144" s="64"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A145" s="64"/>
       <c r="B145" s="88"/>
       <c r="C145" s="88"/>
@@ -5208,7 +5219,7 @@
       <c r="G145" s="64"/>
       <c r="H145" s="64"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A146" s="64"/>
       <c r="B146" s="88"/>
       <c r="C146" s="88"/>
@@ -5218,7 +5229,7 @@
       <c r="G146" s="64"/>
       <c r="H146" s="64"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A147" s="64"/>
       <c r="B147" s="88"/>
       <c r="C147" s="88"/>
@@ -5228,7 +5239,7 @@
       <c r="G147" s="64"/>
       <c r="H147" s="64"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A148" s="64"/>
       <c r="B148" s="88"/>
       <c r="C148" s="88"/>
@@ -5238,7 +5249,7 @@
       <c r="G148" s="64"/>
       <c r="H148" s="64"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A149" s="64"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -5246,7 +5257,7 @@
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
@@ -5271,27 +5282,27 @@
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.90625" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" customWidth="1"/>
-    <col min="3" max="3" width="21.81640625" customWidth="1"/>
-    <col min="4" max="4" width="6.54296875" customWidth="1"/>
-    <col min="5" max="5" width="5.1796875" customWidth="1"/>
-    <col min="6" max="6" width="33.453125" customWidth="1"/>
+    <col min="1" max="1" width="3.921875" customWidth="1"/>
+    <col min="2" max="2" width="13.07421875" customWidth="1"/>
+    <col min="3" max="3" width="21.84375" customWidth="1"/>
+    <col min="4" max="4" width="6.53515625" customWidth="1"/>
+    <col min="5" max="5" width="5.15234375" customWidth="1"/>
+    <col min="6" max="6" width="33.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="192" t="s">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="195" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="194"/>
-    </row>
-    <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
+      <c r="E2" s="196"/>
+      <c r="F2" s="197"/>
+    </row>
+    <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="33" t="s">
         <v>0</v>
       </c>
@@ -5308,7 +5319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B4" s="24" t="s">
         <v>4</v>
       </c>
@@ -5325,7 +5336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B5" s="24"/>
       <c r="C5" s="3"/>
       <c r="D5" s="6" t="s">
@@ -5338,7 +5349,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B6" s="24"/>
       <c r="C6" s="3"/>
       <c r="D6" s="6" t="s">
@@ -5351,7 +5362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B7" s="24"/>
       <c r="C7" s="3"/>
       <c r="D7" s="6" t="s">
@@ -5364,7 +5375,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B8" s="24"/>
       <c r="C8" s="3"/>
       <c r="D8" s="6" t="s">
@@ -5377,7 +5388,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B9" s="24"/>
       <c r="C9" s="3"/>
       <c r="D9" s="6" t="s">
@@ -5390,7 +5401,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B10" s="24"/>
       <c r="C10" s="3"/>
       <c r="D10" s="7"/>
@@ -5399,7 +5410,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B11" s="23" t="s">
         <v>16</v>
       </c>
@@ -5416,7 +5427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B12" s="24"/>
       <c r="C12" s="3"/>
       <c r="D12" s="6" t="s">
@@ -5429,7 +5440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B13" s="24"/>
       <c r="C13" s="3"/>
       <c r="D13" s="6" t="s">
@@ -5442,7 +5453,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B14" s="24"/>
       <c r="C14" s="3"/>
       <c r="D14" s="6" t="s">
@@ -5455,7 +5466,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B15" s="24"/>
       <c r="C15" s="3"/>
       <c r="D15" s="6" t="s">
@@ -5468,7 +5479,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B16" s="24"/>
       <c r="C16" s="3"/>
       <c r="D16" s="6" t="s">
@@ -5481,7 +5492,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B17" s="25"/>
       <c r="C17" s="4"/>
       <c r="D17" s="7"/>
@@ -5490,7 +5501,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B18" s="23" t="s">
         <v>96</v>
       </c>
@@ -5507,7 +5518,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B19" s="30"/>
       <c r="C19" s="4"/>
       <c r="D19" s="32"/>
@@ -5516,7 +5527,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B20" s="22" t="s">
         <v>18</v>
       </c>
@@ -5533,7 +5544,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B21" s="22" t="s">
         <v>21</v>
       </c>
@@ -5550,7 +5561,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B22" s="22" t="s">
         <v>100</v>
       </c>
@@ -5567,7 +5578,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B23" s="22" t="s">
         <v>101</v>
       </c>
@@ -5584,7 +5595,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B24" s="162" t="s">
         <v>37</v>
       </c>
@@ -5601,7 +5612,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B25" s="162" t="s">
         <v>40</v>
       </c>
@@ -5618,7 +5629,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B26" s="162" t="s">
         <v>43</v>
       </c>
@@ -5635,7 +5646,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B27" s="162" t="s">
         <v>51</v>
       </c>
@@ -5652,7 +5663,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B28" s="162" t="s">
         <v>50</v>
       </c>
@@ -5669,7 +5680,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B29" s="163" t="s">
         <v>77</v>
       </c>
@@ -5686,7 +5697,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B30" s="164"/>
       <c r="C30" s="26"/>
       <c r="D30" s="27"/>
@@ -5705,33 +5716,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CD7B95-A2AF-46FE-AB85-2A0D672A14B1}">
-  <dimension ref="A1:F130"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B125" sqref="B125:C127"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K125" sqref="K125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="24.08984375" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" customWidth="1"/>
-    <col min="6" max="6" width="29.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.23046875" customWidth="1"/>
+    <col min="3" max="3" width="24.07421875" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.23046875" customWidth="1"/>
+    <col min="6" max="6" width="29.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="192" t="s">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="195" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="194"/>
-    </row>
-    <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
+      <c r="E2" s="196"/>
+      <c r="F2" s="197"/>
+    </row>
+    <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="33" t="s">
         <v>0</v>
       </c>
@@ -5748,7 +5759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B4" s="24" t="s">
         <v>4</v>
       </c>
@@ -5765,7 +5776,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B5" s="24"/>
       <c r="C5" s="3"/>
       <c r="D5" s="6" t="s">
@@ -5778,7 +5789,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B6" s="24"/>
       <c r="C6" s="3"/>
       <c r="D6" s="6" t="s">
@@ -5791,7 +5802,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B7" s="24"/>
       <c r="C7" s="3"/>
       <c r="D7" s="6" t="s">
@@ -5804,7 +5815,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B8" s="24"/>
       <c r="C8" s="3"/>
       <c r="D8" s="6" t="s">
@@ -5817,7 +5828,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B9" s="24"/>
       <c r="C9" s="3"/>
       <c r="D9" s="6" t="s">
@@ -5830,7 +5841,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B10" s="24"/>
       <c r="C10" s="3"/>
       <c r="D10" s="6" t="s">
@@ -5843,7 +5854,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B11" s="24"/>
       <c r="C11" s="3"/>
       <c r="D11" s="6" t="s">
@@ -5856,7 +5867,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B12" s="24"/>
       <c r="C12" s="3"/>
       <c r="D12" s="6" t="s">
@@ -5869,7 +5880,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B13" s="24"/>
       <c r="C13" s="3"/>
       <c r="D13" s="6" t="s">
@@ -5882,7 +5893,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B14" s="24"/>
       <c r="C14" s="3"/>
       <c r="D14" s="6" t="s">
@@ -5895,7 +5906,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B15" s="24"/>
       <c r="C15" s="3"/>
       <c r="D15" s="7"/>
@@ -5904,7 +5915,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B16" s="23" t="s">
         <v>16</v>
       </c>
@@ -5921,7 +5932,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B17" s="24"/>
       <c r="C17" s="3"/>
       <c r="D17" s="6" t="s">
@@ -5934,7 +5945,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B18" s="24"/>
       <c r="C18" s="3"/>
       <c r="D18" s="6" t="s">
@@ -5947,7 +5958,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B19" s="24"/>
       <c r="C19" s="3"/>
       <c r="D19" s="6" t="s">
@@ -5960,7 +5971,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B20" s="24"/>
       <c r="C20" s="3"/>
       <c r="D20" s="6" t="s">
@@ -5973,7 +5984,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B21" s="24"/>
       <c r="C21" s="3"/>
       <c r="D21" s="6" t="s">
@@ -5986,7 +5997,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B22" s="24"/>
       <c r="C22" s="3"/>
       <c r="D22" s="6" t="s">
@@ -5999,7 +6010,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B23" s="24"/>
       <c r="C23" s="3"/>
       <c r="D23" s="6" t="s">
@@ -6012,7 +6023,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B24" s="24"/>
       <c r="C24" s="3"/>
       <c r="D24" s="6" t="s">
@@ -6025,7 +6036,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B25" s="24"/>
       <c r="C25" s="3"/>
       <c r="D25" s="7"/>
@@ -6034,7 +6045,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B26" s="23" t="s">
         <v>17</v>
       </c>
@@ -6051,7 +6062,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B27" s="24"/>
       <c r="C27" s="3"/>
       <c r="D27" s="6" t="s">
@@ -6064,7 +6075,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B28" s="24"/>
       <c r="C28" s="3"/>
       <c r="D28" s="6" t="s">
@@ -6077,7 +6088,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B29" s="24"/>
       <c r="C29" s="3"/>
       <c r="D29" s="6" t="s">
@@ -6090,7 +6101,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B30" s="24"/>
       <c r="C30" s="3"/>
       <c r="D30" s="6" t="s">
@@ -6103,7 +6114,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B31" s="24"/>
       <c r="C31" s="3"/>
       <c r="D31" s="6" t="s">
@@ -6116,7 +6127,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B32" s="24"/>
       <c r="C32" s="3"/>
       <c r="D32" s="6" t="s">
@@ -6129,7 +6140,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B33" s="24"/>
       <c r="C33" s="3"/>
       <c r="D33" s="6" t="s">
@@ -6142,7 +6153,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B34" s="24"/>
       <c r="C34" s="3"/>
       <c r="D34" s="6" t="s">
@@ -6155,7 +6166,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B35" s="24"/>
       <c r="C35" s="3"/>
       <c r="D35" s="7"/>
@@ -6164,7 +6175,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B36" s="23" t="s">
         <v>18</v>
       </c>
@@ -6181,7 +6192,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B37" s="24"/>
       <c r="C37" s="3"/>
       <c r="D37" s="6" t="s">
@@ -6194,7 +6205,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B38" s="24"/>
       <c r="C38" s="3"/>
       <c r="D38" s="6" t="s">
@@ -6207,7 +6218,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B39" s="24"/>
       <c r="C39" s="3"/>
       <c r="D39" s="6" t="s">
@@ -6220,7 +6231,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B40" s="24"/>
       <c r="C40" s="3"/>
       <c r="D40" s="6" t="s">
@@ -6233,7 +6244,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B41" s="24"/>
       <c r="C41" s="3"/>
       <c r="D41" s="6" t="s">
@@ -6246,7 +6257,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B42" s="24"/>
       <c r="C42" s="3"/>
       <c r="D42" s="6" t="s">
@@ -6259,7 +6270,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B43" s="24"/>
       <c r="C43" s="3"/>
       <c r="D43" s="6" t="s">
@@ -6272,7 +6283,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B44" s="24"/>
       <c r="C44" s="3"/>
       <c r="D44" s="6" t="s">
@@ -6285,7 +6296,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B45" s="36"/>
       <c r="C45" s="26"/>
       <c r="D45" s="27"/>
@@ -6294,7 +6305,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B46" s="24" t="s">
         <v>21</v>
       </c>
@@ -6311,7 +6322,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B47" s="24"/>
       <c r="C47" s="3"/>
       <c r="D47" s="6" t="s">
@@ -6324,7 +6335,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B48" s="24"/>
       <c r="C48" s="3"/>
       <c r="D48" s="6" t="s">
@@ -6337,7 +6348,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B49" s="24"/>
       <c r="C49" s="3"/>
       <c r="D49" s="6" t="s">
@@ -6350,7 +6361,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B50" s="24"/>
       <c r="C50" s="3"/>
       <c r="D50" s="6" t="s">
@@ -6363,7 +6374,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B51" s="24"/>
       <c r="C51" s="3"/>
       <c r="D51" s="6" t="s">
@@ -6376,7 +6387,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B52" s="24"/>
       <c r="C52" s="3"/>
       <c r="D52" s="6" t="s">
@@ -6389,7 +6400,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B53" s="24"/>
       <c r="C53" s="3"/>
       <c r="D53" s="6" t="s">
@@ -6402,7 +6413,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B54" s="24"/>
       <c r="C54" s="3"/>
       <c r="D54" s="6" t="s">
@@ -6415,7 +6426,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B55" s="24"/>
       <c r="C55" s="3"/>
       <c r="D55" s="6" t="s">
@@ -6428,7 +6439,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B56" s="24"/>
       <c r="C56" s="3"/>
       <c r="D56" s="6" t="s">
@@ -6441,7 +6452,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B57" s="24"/>
       <c r="C57" s="3"/>
       <c r="D57" s="7"/>
@@ -6450,7 +6461,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B58" s="23" t="s">
         <v>24</v>
       </c>
@@ -6467,7 +6478,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B59" s="24"/>
       <c r="C59" s="3"/>
       <c r="D59" s="6" t="s">
@@ -6480,7 +6491,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B60" s="24"/>
       <c r="C60" s="3"/>
       <c r="D60" s="6" t="s">
@@ -6493,7 +6504,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B61" s="24"/>
       <c r="C61" s="3"/>
       <c r="D61" s="6" t="s">
@@ -6506,7 +6517,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B62" s="24"/>
       <c r="C62" s="3"/>
       <c r="D62" s="6" t="s">
@@ -6519,7 +6530,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B63" s="24"/>
       <c r="C63" s="3"/>
       <c r="D63" s="6" t="s">
@@ -6532,7 +6543,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B64" s="24"/>
       <c r="C64" s="3"/>
       <c r="D64" s="6" t="s">
@@ -6545,7 +6556,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B65" s="24"/>
       <c r="C65" s="3"/>
       <c r="D65" s="6" t="s">
@@ -6558,7 +6569,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B66" s="24"/>
       <c r="C66" s="3"/>
       <c r="D66" s="6" t="s">
@@ -6571,7 +6582,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B67" s="24"/>
       <c r="C67" s="3"/>
       <c r="D67" s="7"/>
@@ -6580,7 +6591,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B68" s="23" t="s">
         <v>177</v>
       </c>
@@ -6597,7 +6608,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B69" s="24"/>
       <c r="C69" s="3"/>
       <c r="D69" s="6" t="s">
@@ -6610,7 +6621,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B70" s="24"/>
       <c r="C70" s="3"/>
       <c r="D70" s="6" t="s">
@@ -6623,7 +6634,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B71" s="24"/>
       <c r="C71" s="3"/>
       <c r="D71" s="6" t="s">
@@ -6636,7 +6647,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B72" s="24"/>
       <c r="C72" s="3"/>
       <c r="D72" s="6" t="s">
@@ -6649,7 +6660,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B73" s="24"/>
       <c r="C73" s="3"/>
       <c r="D73" s="6" t="s">
@@ -6662,7 +6673,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B74" s="24"/>
       <c r="C74" s="3"/>
       <c r="D74" s="6" t="s">
@@ -6675,7 +6686,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B75" s="24"/>
       <c r="C75" s="3"/>
       <c r="D75" s="6" t="s">
@@ -6688,7 +6699,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B76" s="24"/>
       <c r="C76" s="3"/>
       <c r="D76" s="6" t="s">
@@ -6701,7 +6712,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B77" s="24"/>
       <c r="C77" s="3"/>
       <c r="D77" s="7"/>
@@ -6710,7 +6721,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B78" s="23" t="s">
         <v>101</v>
       </c>
@@ -6727,7 +6738,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B79" s="24"/>
       <c r="C79" s="3"/>
       <c r="D79" s="6" t="s">
@@ -6740,7 +6751,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B80" s="24"/>
       <c r="C80" s="3"/>
       <c r="D80" s="6" t="s">
@@ -6753,7 +6764,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B81" s="24"/>
       <c r="C81" s="3"/>
       <c r="D81" s="6" t="s">
@@ -6766,7 +6777,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B82" s="24"/>
       <c r="C82" s="3"/>
       <c r="D82" s="6" t="s">
@@ -6779,7 +6790,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B83" s="24"/>
       <c r="C83" s="3"/>
       <c r="D83" s="6" t="s">
@@ -6792,7 +6803,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B84" s="24"/>
       <c r="C84" s="3"/>
       <c r="D84" s="6" t="s">
@@ -6805,7 +6816,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B85" s="24"/>
       <c r="C85" s="3"/>
       <c r="D85" s="6" t="s">
@@ -6818,7 +6829,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B86" s="24"/>
       <c r="C86" s="3"/>
       <c r="D86" s="6" t="s">
@@ -6831,7 +6842,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B87" s="25"/>
       <c r="C87" s="4"/>
       <c r="D87" s="7"/>
@@ -6840,7 +6851,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B88" s="25" t="s">
         <v>31</v>
       </c>
@@ -6857,7 +6868,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B89" s="22" t="s">
         <v>182</v>
       </c>
@@ -6874,7 +6885,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B90" s="22" t="s">
         <v>188</v>
       </c>
@@ -6891,7 +6902,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B91" s="22" t="s">
         <v>189</v>
       </c>
@@ -6908,7 +6919,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B92" s="22" t="s">
         <v>190</v>
       </c>
@@ -6925,7 +6936,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B93" s="22" t="s">
         <v>193</v>
       </c>
@@ -6942,7 +6953,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B94" s="45" t="s">
         <v>37</v>
       </c>
@@ -6959,7 +6970,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B95" s="117"/>
       <c r="C95" s="64"/>
       <c r="D95" s="48"/>
@@ -6968,7 +6979,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B96" s="117"/>
       <c r="C96" s="64"/>
       <c r="D96" s="48" t="s">
@@ -6981,7 +6992,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B97" s="117"/>
       <c r="C97" s="64"/>
       <c r="D97" s="48"/>
@@ -6990,7 +7001,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B98" s="117"/>
       <c r="C98" s="64"/>
       <c r="D98" s="48" t="s">
@@ -7003,7 +7014,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B99" s="117"/>
       <c r="C99" s="64"/>
       <c r="D99" s="48"/>
@@ -7012,7 +7023,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B100" s="117"/>
       <c r="C100" s="64"/>
       <c r="D100" s="48"/>
@@ -7023,7 +7034,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B101" s="117"/>
       <c r="C101" s="64"/>
       <c r="D101" s="48"/>
@@ -7032,7 +7043,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B102" s="117"/>
       <c r="C102" s="64"/>
       <c r="D102" s="48"/>
@@ -7043,7 +7054,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B103" s="117"/>
       <c r="C103" s="64"/>
       <c r="D103" s="48"/>
@@ -7052,7 +7063,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B104" s="117"/>
       <c r="C104" s="64"/>
       <c r="D104" s="48"/>
@@ -7063,7 +7074,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B105" s="117"/>
       <c r="C105" s="64"/>
       <c r="D105" s="48"/>
@@ -7072,7 +7083,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B106" s="117"/>
       <c r="C106" s="64"/>
       <c r="D106" s="48" t="s">
@@ -7085,7 +7096,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B107" s="118"/>
       <c r="C107" s="64"/>
       <c r="D107" s="48"/>
@@ -7094,7 +7105,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B108" s="52" t="s">
         <v>40</v>
       </c>
@@ -7111,7 +7122,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B109" s="52" t="s">
         <v>43</v>
       </c>
@@ -7128,7 +7139,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B110" s="52" t="s">
         <v>51</v>
       </c>
@@ -7145,7 +7156,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B111" s="52" t="s">
         <v>50</v>
       </c>
@@ -7162,7 +7173,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B112" s="52" t="s">
         <v>77</v>
       </c>
@@ -7179,7 +7190,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B113" s="52" t="s">
         <v>219</v>
       </c>
@@ -7196,7 +7207,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B114" s="52" t="s">
         <v>220</v>
       </c>
@@ -7213,7 +7224,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B115" s="52" t="s">
         <v>56</v>
       </c>
@@ -7230,7 +7241,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B116" s="52" t="s">
         <v>57</v>
       </c>
@@ -7247,7 +7258,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B117" s="52" t="s">
         <v>58</v>
       </c>
@@ -7264,7 +7275,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B118" s="65" t="s">
         <v>59</v>
       </c>
@@ -7281,7 +7292,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B119" s="66"/>
       <c r="C119" s="58"/>
       <c r="D119" s="59" t="s">
@@ -7294,7 +7305,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B120" s="65" t="s">
         <v>60</v>
       </c>
@@ -7311,7 +7322,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B121" s="66"/>
       <c r="C121" s="58"/>
       <c r="D121" s="59" t="s">
@@ -7324,7 +7335,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B122" s="52" t="s">
         <v>65</v>
       </c>
@@ -7341,7 +7352,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B123" s="65" t="s">
         <v>66</v>
       </c>
@@ -7358,10 +7369,10 @@
         <v>259</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B124" s="185"/>
-      <c r="C124" s="186"/>
-      <c r="D124" s="59" t="s">
+      <c r="C124" s="189"/>
+      <c r="D124" s="48" t="s">
         <v>32</v>
       </c>
       <c r="E124" s="44" t="s">
@@ -7371,91 +7382,108 @@
         <v>260</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A125" s="64"/>
-      <c r="B125" s="89" t="s">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B125" s="190" t="s">
+        <v>67</v>
+      </c>
+      <c r="C125" s="188" t="s">
+        <v>478</v>
+      </c>
+      <c r="D125" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="E125" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F125" s="129" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A126" s="64"/>
+      <c r="B126" s="87" t="s">
         <v>343</v>
       </c>
-      <c r="C125" s="102" t="s">
+      <c r="C126" s="97" t="s">
         <v>344</v>
       </c>
-      <c r="D125" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="E125" s="140" t="s">
+      <c r="D126" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E126" s="40" t="s">
         <v>186</v>
       </c>
-      <c r="F125" s="115" t="s">
+      <c r="F126" s="108" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A126" s="64"/>
-      <c r="B126" s="93"/>
-      <c r="C126" s="131"/>
-      <c r="D126" s="138"/>
-      <c r="E126" s="126"/>
-      <c r="F126" s="127" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A127" s="64"/>
       <c r="B127" s="93"/>
-      <c r="C127" s="56"/>
-      <c r="D127" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="E127" s="126" t="s">
-        <v>197</v>
-      </c>
+      <c r="C127" s="131"/>
+      <c r="D127" s="138"/>
+      <c r="E127" s="38"/>
       <c r="F127" s="127" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A128" s="64"/>
       <c r="B128" s="93"/>
-      <c r="C128" s="133"/>
-      <c r="D128" s="139"/>
-      <c r="E128" s="135"/>
-      <c r="F128" s="128" t="s">
+      <c r="C128" s="56"/>
+      <c r="D128" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E128" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="F128" s="127" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A129" s="64"/>
+      <c r="B129" s="93"/>
+      <c r="C129" s="133"/>
+      <c r="D129" s="139"/>
+      <c r="E129" s="39"/>
+      <c r="F129" s="128" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A129" s="64"/>
-      <c r="B129" s="92" t="s">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A130" s="64"/>
+      <c r="B130" s="92" t="s">
         <v>349</v>
       </c>
-      <c r="C129" s="132" t="s">
+      <c r="C130" s="132" t="s">
         <v>351</v>
       </c>
-      <c r="D129" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="E129" s="136" t="s">
+      <c r="D130" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="E130" s="40" t="s">
         <v>350</v>
       </c>
-      <c r="F129" s="129" t="s">
+      <c r="F130" s="129" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="64"/>
-      <c r="B130" s="94" t="s">
+    <row r="131" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A131" s="64"/>
+      <c r="B131" s="94" t="s">
         <v>353</v>
       </c>
-      <c r="C130" s="134" t="s">
+      <c r="C131" s="134" t="s">
         <v>354</v>
       </c>
-      <c r="D130" s="95" t="s">
-        <v>32</v>
-      </c>
-      <c r="E130" s="137" t="s">
+      <c r="D131" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="E131" s="191" t="s">
         <v>350</v>
       </c>
-      <c r="F130" s="130" t="s">
+      <c r="F131" s="130" t="s">
         <v>355</v>
       </c>
     </row>
@@ -7476,16 +7504,16 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.90625" customWidth="1"/>
-    <col min="2" max="2" width="33.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="1" max="1" width="2.921875" customWidth="1"/>
+    <col min="2" max="2" width="33.61328125" customWidth="1"/>
+    <col min="3" max="3" width="12.69140625" customWidth="1"/>
+    <col min="4" max="4" width="6.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="172" t="s">
         <v>446</v>
       </c>
@@ -7496,7 +7524,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="175" t="s">
         <v>455</v>
       </c>
@@ -7507,7 +7535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" ht="46" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="176" t="s">
         <v>456</v>
       </c>
@@ -7518,7 +7546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="177" t="s">
         <v>458</v>
       </c>
@@ -7529,7 +7557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" ht="56.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B6" s="178" t="s">
         <v>457</v>
       </c>
@@ -7540,7 +7568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B7" s="182" t="s">
         <v>454</v>
       </c>
@@ -7562,18 +7590,18 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="5.90625" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" customWidth="1"/>
-    <col min="7" max="7" width="6.90625" customWidth="1"/>
-    <col min="8" max="8" width="16.26953125" customWidth="1"/>
+    <col min="2" max="2" width="5.921875" customWidth="1"/>
+    <col min="3" max="3" width="9.23046875" customWidth="1"/>
+    <col min="5" max="5" width="13.61328125" customWidth="1"/>
+    <col min="6" max="6" width="13.69140625" customWidth="1"/>
+    <col min="7" max="7" width="6.921875" customWidth="1"/>
+    <col min="8" max="8" width="16.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E2" s="70" t="s">
         <v>241</v>
       </c>
@@ -7587,7 +7615,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E3" s="67">
         <v>22050</v>
       </c>
@@ -7602,13 +7630,13 @@
         <v>1073741824</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E4" s="55"/>
       <c r="F4" s="55"/>
       <c r="G4" s="55"/>
       <c r="H4" s="55"/>
     </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="70" t="s">
         <v>261</v>
       </c>
@@ -7625,7 +7653,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B6" s="75"/>
       <c r="C6" s="73">
         <v>0</v>
@@ -7643,7 +7671,7 @@
         <v>0x3ACCCC</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B7" s="75"/>
       <c r="C7" s="73">
         <v>1</v>
@@ -7661,7 +7689,7 @@
         <v>0x3E4BE2</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" s="75"/>
       <c r="C8" s="73">
         <v>2</v>
@@ -7679,7 +7707,7 @@
         <v>0x420032</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B9" s="75"/>
       <c r="C9" s="73">
         <v>3</v>
@@ -7697,7 +7725,7 @@
         <v>0x45ECE5</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B10" s="75"/>
       <c r="C10" s="73">
         <v>4</v>
@@ -7715,7 +7743,7 @@
         <v>0x4A1556</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B11" s="75"/>
       <c r="C11" s="73">
         <v>5</v>
@@ -7733,7 +7761,7 @@
         <v>0x4E7D13</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B12" s="75"/>
       <c r="C12" s="73">
         <v>6</v>
@@ -7751,7 +7779,7 @@
         <v>0x5327DF</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B13" s="75"/>
       <c r="C13" s="73">
         <v>7</v>
@@ -7769,7 +7797,7 @@
         <v>0x5819B7</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B14" s="75"/>
       <c r="C14" s="73">
         <v>8</v>
@@ -7787,7 +7815,7 @@
         <v>0x5D56D4</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B15" s="75"/>
       <c r="C15" s="73">
         <v>9</v>
@@ -7805,7 +7833,7 @@
         <v>0x62E3B0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B16" s="75"/>
       <c r="C16" s="73">
         <v>10</v>
@@ -7823,7 +7851,7 @@
         <v>0x68C50A</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B17" s="75"/>
       <c r="C17" s="73">
         <v>11</v>
@@ -7841,7 +7869,7 @@
         <v>0x6EFFE7</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B18" s="75"/>
       <c r="C18" s="73">
         <v>12</v>
@@ -7859,7 +7887,7 @@
         <v>0x759999</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B19" s="75"/>
       <c r="C19" s="73">
         <v>13</v>
@@ -7877,7 +7905,7 @@
         <v>0x7C97C5</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B20" s="75"/>
       <c r="C20" s="73">
         <v>14</v>
@@ -7895,7 +7923,7 @@
         <v>0x840064</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B21" s="75"/>
       <c r="C21" s="73">
         <v>15</v>
@@ -7913,7 +7941,7 @@
         <v>0x8BD9CB</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B22" s="75"/>
       <c r="C22" s="73">
         <v>16</v>
@@ -7931,7 +7959,7 @@
         <v>0x942AAD</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B23" s="75"/>
       <c r="C23" s="73">
         <v>17</v>
@@ -7949,7 +7977,7 @@
         <v>0x9CFA27</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B24" s="75"/>
       <c r="C24" s="73">
         <v>18</v>
@@ -7967,7 +7995,7 @@
         <v>0xA64FBF</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B25" s="75"/>
       <c r="C25" s="73">
         <v>19</v>
@@ -7985,7 +8013,7 @@
         <v>0xB0336E</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B26" s="75"/>
       <c r="C26" s="73">
         <v>20</v>
@@ -8003,7 +8031,7 @@
         <v>0xBAADA9</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B27" s="78"/>
       <c r="C27" s="74">
         <v>21</v>
@@ -8021,7 +8049,7 @@
         <v>0xC5C761</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B28" s="78"/>
       <c r="C28" s="74">
         <v>22</v>
@@ -8039,7 +8067,7 @@
         <v>0xD18A14</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B29" s="78"/>
       <c r="C29" s="74">
         <v>23</v>
@@ -8057,7 +8085,7 @@
         <v>0xDDFFCE</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B30" s="78" t="s">
         <v>233</v>
       </c>
@@ -8077,7 +8105,7 @@
         <v>0xEB3333</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B31" s="78"/>
       <c r="C31" s="74">
         <v>25</v>
@@ -8095,7 +8123,7 @@
         <v>0xF92F8B</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B32" s="78"/>
       <c r="C32" s="74">
         <v>26</v>
@@ -8113,7 +8141,7 @@
         <v>0x10800C9</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B33" s="78"/>
       <c r="C33" s="74">
         <v>27</v>
@@ -8131,7 +8159,7 @@
         <v>0x117B396</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B34" s="78"/>
       <c r="C34" s="74">
         <v>28</v>
@@ -8149,7 +8177,7 @@
         <v>0x128555B</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B35" s="78"/>
       <c r="C35" s="74">
         <v>29</v>
@@ -8167,7 +8195,7 @@
         <v>0x139F44F</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B36" s="78"/>
       <c r="C36" s="74">
         <v>30</v>
@@ -8185,7 +8213,7 @@
         <v>0x14C9F7E</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B37" s="78"/>
       <c r="C37" s="74">
         <v>31</v>
@@ -8203,7 +8231,7 @@
         <v>0x16066DD</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B38" s="78"/>
       <c r="C38" s="74">
         <v>32</v>
@@ -8221,7 +8249,7 @@
         <v>0x1755B52</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B39" s="78"/>
       <c r="C39" s="74">
         <v>33</v>
@@ -8239,7 +8267,7 @@
         <v>0x18B8EC3</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B40" s="78"/>
       <c r="C40" s="74">
         <v>34</v>
@@ -8257,7 +8285,7 @@
         <v>0x1A31429</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B41" s="78"/>
       <c r="C41" s="74">
         <v>35</v>
@@ -8275,7 +8303,7 @@
         <v>0x1BBFF9C</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B42" s="80" t="s">
         <v>235</v>
       </c>
@@ -8295,7 +8323,7 @@
         <v>0x1D66666</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B43" s="80"/>
       <c r="C43" s="81">
         <v>37</v>
@@ -8313,7 +8341,7 @@
         <v>0x1F25F16</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B44" s="80"/>
       <c r="C44" s="81">
         <v>38</v>
@@ -8331,7 +8359,7 @@
         <v>0x2100192</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B45" s="80"/>
       <c r="C45" s="81">
         <v>39</v>
@@ -8349,7 +8377,7 @@
         <v>0x22F672C</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B46" s="80"/>
       <c r="C46" s="81">
         <v>40</v>
@@ -8367,7 +8395,7 @@
         <v>0x250AAB7</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B47" s="80"/>
       <c r="C47" s="81">
         <v>41</v>
@@ -8385,7 +8413,7 @@
         <v>0x273E89E</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B48" s="80"/>
       <c r="C48" s="81">
         <v>42</v>
@@ -8403,7 +8431,7 @@
         <v>0x2993EFD</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B49" s="80"/>
       <c r="C49" s="81">
         <v>43</v>
@@ -8421,7 +8449,7 @@
         <v>0x2C0CDBB</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B50" s="80"/>
       <c r="C50" s="81">
         <v>44</v>
@@ -8439,7 +8467,7 @@
         <v>0x2EAB6A4</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B51" s="80"/>
       <c r="C51" s="81">
         <v>45</v>
@@ -8457,7 +8485,7 @@
         <v>0x3171D87</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B52" s="80"/>
       <c r="C52" s="81">
         <v>46</v>
@@ -8475,7 +8503,7 @@
         <v>0x3462852</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B53" s="80"/>
       <c r="C53" s="81">
         <v>47</v>
@@ -8493,7 +8521,7 @@
         <v>0x377FF38</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B54" s="80" t="s">
         <v>234</v>
       </c>
@@ -8513,7 +8541,7 @@
         <v>0x3ACCCCC</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B55" s="80"/>
       <c r="C55" s="81">
         <v>49</v>
@@ -8531,7 +8559,7 @@
         <v>0x3E4BE2D</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B56" s="80"/>
       <c r="C56" s="81">
         <v>50</v>
@@ -8549,7 +8577,7 @@
         <v>0x4200325</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B57" s="80"/>
       <c r="C57" s="81">
         <v>51</v>
@@ -8567,7 +8595,7 @@
         <v>0x45ECE59</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B58" s="80"/>
       <c r="C58" s="81">
         <v>52</v>
@@ -8585,7 +8613,7 @@
         <v>0x4A1556E</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B59" s="80"/>
       <c r="C59" s="81">
         <v>53</v>
@@ -8603,7 +8631,7 @@
         <v>0x4E7D13C</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B60" s="80"/>
       <c r="C60" s="81">
         <v>54</v>
@@ -8621,7 +8649,7 @@
         <v>0x5327DFB</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B61" s="80"/>
       <c r="C61" s="81">
         <v>55</v>
@@ -8639,7 +8667,7 @@
         <v>0x5819B77</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B62" s="80"/>
       <c r="C62" s="81">
         <v>56</v>
@@ -8657,7 +8685,7 @@
         <v>0x5D56D49</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B63" s="80"/>
       <c r="C63" s="81">
         <v>57</v>
@@ -8675,7 +8703,7 @@
         <v>0x62E3B0E</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B64" s="80"/>
       <c r="C64" s="81">
         <v>58</v>
@@ -8693,7 +8721,7 @@
         <v>0x68C50A5</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B65" s="80"/>
       <c r="C65" s="81">
         <v>59</v>
@@ -8711,7 +8739,7 @@
         <v>0x6EFFE70</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B66" s="80" t="s">
         <v>236</v>
       </c>
@@ -8731,7 +8759,7 @@
         <v>0x7599999</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B67" s="80"/>
       <c r="C67" s="81">
         <v>61</v>
@@ -8749,7 +8777,7 @@
         <v>0x7C97C5A</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B68" s="80"/>
       <c r="C68" s="81">
         <v>62</v>
@@ -8767,7 +8795,7 @@
         <v>0x840064B</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B69" s="80"/>
       <c r="C69" s="81">
         <v>63</v>
@@ -8785,7 +8813,7 @@
         <v>0x8BD9CB3</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B70" s="80"/>
       <c r="C70" s="81">
         <v>64</v>
@@ -8803,7 +8831,7 @@
         <v>0x942AADD</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B71" s="80"/>
       <c r="C71" s="81">
         <v>65</v>
@@ -8821,7 +8849,7 @@
         <v>0x9CFA279</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B72" s="80"/>
       <c r="C72" s="81">
         <v>66</v>
@@ -8839,7 +8867,7 @@
         <v>0xA64FBF7</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B73" s="80"/>
       <c r="C73" s="81">
         <v>67</v>
@@ -8857,7 +8885,7 @@
         <v>0xB0336EF</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B74" s="80"/>
       <c r="C74" s="81">
         <v>68</v>
@@ -8875,7 +8903,7 @@
         <v>0xBAADA93</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B75" s="80"/>
       <c r="C75" s="81">
         <v>69</v>
@@ -8893,7 +8921,7 @@
         <v>0xC5C761D</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B76" s="80"/>
       <c r="C76" s="81">
         <v>70</v>
@@ -8911,7 +8939,7 @@
         <v>0xD18A14B</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B77" s="80"/>
       <c r="C77" s="81">
         <v>71</v>
@@ -8929,7 +8957,7 @@
         <v>0xDDFFCE1</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B78" s="80" t="s">
         <v>237</v>
       </c>
@@ -8949,7 +8977,7 @@
         <v>0xEB33333</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B79" s="80"/>
       <c r="C79" s="81">
         <v>73</v>
@@ -8967,7 +8995,7 @@
         <v>0xF92F8B5</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B80" s="80"/>
       <c r="C80" s="81">
         <v>74</v>
@@ -8985,7 +9013,7 @@
         <v>0x10800C97</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B81" s="80"/>
       <c r="C81" s="81">
         <v>75</v>
@@ -9003,7 +9031,7 @@
         <v>0x117B3966</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B82" s="80"/>
       <c r="C82" s="81">
         <v>76</v>
@@ -9021,7 +9049,7 @@
         <v>0x128555BB</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B83" s="80"/>
       <c r="C83" s="81">
         <v>77</v>
@@ -9039,7 +9067,7 @@
         <v>0x139F44F3</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B84" s="80"/>
       <c r="C84" s="81">
         <v>78</v>
@@ -9057,7 +9085,7 @@
         <v>0x14C9F7EE</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B85" s="80"/>
       <c r="C85" s="81">
         <v>79</v>
@@ -9075,7 +9103,7 @@
         <v>0x16066DDF</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B86" s="80"/>
       <c r="C86" s="81">
         <v>80</v>
@@ -9093,7 +9121,7 @@
         <v>0x1755B527</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B87" s="80"/>
       <c r="C87" s="81">
         <v>81</v>
@@ -9111,7 +9139,7 @@
         <v>0x18B8EC3B</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B88" s="80"/>
       <c r="C88" s="81">
         <v>82</v>
@@ -9129,7 +9157,7 @@
         <v>0x1A314296</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B89" s="80"/>
       <c r="C89" s="81">
         <v>83</v>
@@ -9147,7 +9175,7 @@
         <v>0x1BBFF9C2</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B90" s="80" t="s">
         <v>239</v>
       </c>
@@ -9167,7 +9195,7 @@
         <v>0x1D666666</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B91" s="80"/>
       <c r="C91" s="81">
         <v>85</v>
@@ -9185,7 +9213,7 @@
         <v>0x1F25F16A</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B92" s="80"/>
       <c r="C92" s="81">
         <v>86</v>
@@ -9203,7 +9231,7 @@
         <v>0x2100192E</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B93" s="80"/>
       <c r="C93" s="81">
         <v>87</v>
@@ -9221,7 +9249,7 @@
         <v>0x22F672CC</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B94" s="80"/>
       <c r="C94" s="81">
         <v>88</v>
@@ -9239,7 +9267,7 @@
         <v>0x250AAB77</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B95" s="80"/>
       <c r="C95" s="81">
         <v>89</v>
@@ -9257,7 +9285,7 @@
         <v>0x273E89E6</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B96" s="80"/>
       <c r="C96" s="81">
         <v>90</v>
@@ -9275,7 +9303,7 @@
         <v>0x2993EFDC</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B97" s="80"/>
       <c r="C97" s="81">
         <v>91</v>
@@ -9293,7 +9321,7 @@
         <v>0x2C0CDBBF</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B98" s="80"/>
       <c r="C98" s="81">
         <v>92</v>
@@ -9311,7 +9339,7 @@
         <v>0x2EAB6A4F</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B99" s="80"/>
       <c r="C99" s="81">
         <v>93</v>
@@ -9329,7 +9357,7 @@
         <v>0x3171D876</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B100" s="80"/>
       <c r="C100" s="81">
         <v>94</v>
@@ -9347,7 +9375,7 @@
         <v>0x3462852D</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B101" s="80"/>
       <c r="C101" s="81">
         <v>95</v>
@@ -9365,7 +9393,7 @@
         <v>0x377FF385</v>
       </c>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B102" s="80" t="s">
         <v>238</v>
       </c>
@@ -9385,7 +9413,7 @@
         <v>0x3ACCCCCC</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B103" s="78"/>
       <c r="C103" s="74">
         <v>97</v>
@@ -9403,7 +9431,7 @@
         <v>0x3E4BE2D5</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B104" s="78"/>
       <c r="C104" s="74">
         <v>98</v>
@@ -9421,7 +9449,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B105" s="78"/>
       <c r="C105" s="74">
         <v>99</v>
@@ -9439,7 +9467,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B106" s="78"/>
       <c r="C106" s="74">
         <v>100</v>
@@ -9457,7 +9485,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B107" s="78"/>
       <c r="C107" s="74">
         <v>101</v>
@@ -9475,7 +9503,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B108" s="78"/>
       <c r="C108" s="74">
         <v>102</v>
@@ -9493,7 +9521,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B109" s="78"/>
       <c r="C109" s="74">
         <v>103</v>
@@ -9511,7 +9539,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B110" s="78"/>
       <c r="C110" s="74">
         <v>104</v>
@@ -9529,7 +9557,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B111" s="78"/>
       <c r="C111" s="74">
         <v>105</v>
@@ -9547,7 +9575,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B112" s="78"/>
       <c r="C112" s="74">
         <v>106</v>
@@ -9565,7 +9593,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B113" s="78"/>
       <c r="C113" s="74">
         <v>107</v>
@@ -9583,7 +9611,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B114" s="78" t="s">
         <v>240</v>
       </c>
@@ -9603,7 +9631,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B115" s="75"/>
       <c r="C115" s="73">
         <v>109</v>
@@ -9621,7 +9649,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B116" s="75"/>
       <c r="C116" s="73">
         <v>110</v>
@@ -9639,7 +9667,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B117" s="75"/>
       <c r="C117" s="73">
         <v>111</v>
@@ -9657,7 +9685,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B118" s="75"/>
       <c r="C118" s="73">
         <v>112</v>
@@ -9675,7 +9703,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B119" s="75"/>
       <c r="C119" s="73">
         <v>113</v>
@@ -9693,7 +9721,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B120" s="75"/>
       <c r="C120" s="73">
         <v>114</v>
@@ -9711,7 +9739,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B121" s="75"/>
       <c r="C121" s="73">
         <v>115</v>
@@ -9729,7 +9757,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B122" s="75"/>
       <c r="C122" s="73">
         <v>116</v>
@@ -9747,7 +9775,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B123" s="75"/>
       <c r="C123" s="73">
         <v>117</v>
@@ -9765,7 +9793,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B124" s="75"/>
       <c r="C124" s="73">
         <v>118</v>
@@ -9783,7 +9811,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B125" s="75"/>
       <c r="C125" s="73">
         <v>119</v>
@@ -9801,7 +9829,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B126" s="75"/>
       <c r="C126" s="73">
         <v>120</v>
@@ -9819,7 +9847,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B127" s="75"/>
       <c r="C127" s="73">
         <v>121</v>
@@ -9837,7 +9865,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B128" s="75"/>
       <c r="C128" s="73">
         <v>122</v>
@@ -9855,7 +9883,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B129" s="75"/>
       <c r="C129" s="73">
         <v>123</v>
@@ -9873,7 +9901,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B130" s="75"/>
       <c r="C130" s="73">
         <v>124</v>
@@ -9891,7 +9919,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B131" s="75"/>
       <c r="C131" s="73">
         <v>125</v>
@@ -9909,7 +9937,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B132" s="75"/>
       <c r="C132" s="73">
         <v>126</v>
@@ -9927,7 +9955,7 @@
         <v>0x3FFFFFFF</v>
       </c>
     </row>
-    <row r="133" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="133" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B133" s="77"/>
       <c r="C133" s="68">
         <v>127</v>
@@ -9958,12 +9986,12 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="64"/>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -9980,7 +10008,7 @@
       <c r="N1" s="64"/>
       <c r="O1" s="64"/>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="64"/>
       <c r="B2" s="148" t="s">
         <v>402</v>
@@ -10017,7 +10045,7 @@
       <c r="N2" s="64"/>
       <c r="O2" s="64"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="64"/>
       <c r="B3" s="145" t="s">
         <v>399</v>
@@ -10054,7 +10082,7 @@
       <c r="N3" s="64"/>
       <c r="O3" s="64"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="64"/>
       <c r="B4" s="143" t="s">
         <v>400</v>
@@ -10091,32 +10119,32 @@
       <c r="N4" s="64"/>
       <c r="O4" s="64"/>
     </row>
-    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="64"/>
       <c r="B5" s="144" t="s">
         <v>401</v>
       </c>
-      <c r="C5" s="195" t="s">
+      <c r="C5" s="198" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="195"/>
-      <c r="E5" s="195"/>
-      <c r="F5" s="196" t="s">
+      <c r="D5" s="198"/>
+      <c r="E5" s="198"/>
+      <c r="F5" s="199" t="s">
         <v>398</v>
       </c>
-      <c r="G5" s="196"/>
-      <c r="H5" s="196"/>
-      <c r="I5" s="197" t="s">
+      <c r="G5" s="199"/>
+      <c r="H5" s="199"/>
+      <c r="I5" s="200" t="s">
         <v>403</v>
       </c>
-      <c r="J5" s="197"/>
-      <c r="K5" s="198"/>
+      <c r="J5" s="200"/>
+      <c r="K5" s="201"/>
       <c r="L5" s="64"/>
       <c r="M5" s="64"/>
       <c r="N5" s="64"/>
       <c r="O5" s="64"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="64"/>
       <c r="B6" s="64"/>
       <c r="C6" s="64"/>
@@ -10133,7 +10161,7 @@
       <c r="N6" s="64"/>
       <c r="O6" s="64"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="64"/>
       <c r="B7" s="64"/>
       <c r="C7" s="64"/>
@@ -10150,7 +10178,7 @@
       <c r="N7" s="64"/>
       <c r="O7" s="64"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="64"/>
       <c r="B8" s="64"/>
       <c r="C8" s="64"/>
@@ -10167,7 +10195,7 @@
       <c r="N8" s="64"/>
       <c r="O8" s="64"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="64"/>
       <c r="B9" s="64"/>
       <c r="C9" s="64"/>
@@ -10184,7 +10212,7 @@
       <c r="N9" s="64"/>
       <c r="O9" s="64"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="64"/>
       <c r="B10" s="64"/>
       <c r="C10" s="64"/>
@@ -10201,7 +10229,7 @@
       <c r="N10" s="64"/>
       <c r="O10" s="64"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="64"/>
       <c r="B11" s="64"/>
       <c r="C11" s="64"/>
@@ -10218,7 +10246,7 @@
       <c r="N11" s="64"/>
       <c r="O11" s="64"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="64"/>
       <c r="B12" s="64"/>
       <c r="C12" s="64"/>
@@ -10235,7 +10263,7 @@
       <c r="N12" s="64"/>
       <c r="O12" s="64"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="64"/>
       <c r="B13" s="64"/>
       <c r="C13" s="64"/>
@@ -10252,7 +10280,7 @@
       <c r="N13" s="64"/>
       <c r="O13" s="64"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="64"/>
       <c r="B14" s="64"/>
       <c r="C14" s="64"/>
@@ -10269,7 +10297,7 @@
       <c r="N14" s="64"/>
       <c r="O14" s="64"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="64"/>
       <c r="B15" s="64"/>
       <c r="C15" s="64"/>
@@ -10286,7 +10314,7 @@
       <c r="N15" s="64"/>
       <c r="O15" s="64"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="64"/>
       <c r="B16" s="64"/>
       <c r="C16" s="64"/>
@@ -10303,7 +10331,7 @@
       <c r="N16" s="64"/>
       <c r="O16" s="64"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="64"/>
       <c r="B17" s="64"/>
       <c r="C17" s="64"/>
@@ -10320,7 +10348,7 @@
       <c r="N17" s="64"/>
       <c r="O17" s="64"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" s="64"/>
       <c r="B18" s="64"/>
       <c r="C18" s="64"/>
@@ -10337,7 +10365,7 @@
       <c r="N18" s="64"/>
       <c r="O18" s="64"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" s="64"/>
       <c r="B19" s="64"/>
       <c r="C19" s="64"/>
@@ -10354,7 +10382,7 @@
       <c r="N19" s="64"/>
       <c r="O19" s="64"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" s="64"/>
       <c r="B20" s="64"/>
       <c r="C20" s="64"/>
@@ -10371,7 +10399,7 @@
       <c r="N20" s="64"/>
       <c r="O20" s="64"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" s="64"/>
       <c r="B21" s="64"/>
       <c r="C21" s="64"/>
@@ -10388,7 +10416,7 @@
       <c r="N21" s="64"/>
       <c r="O21" s="64"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" s="64"/>
       <c r="B22" s="64"/>
       <c r="C22" s="64"/>
@@ -10405,7 +10433,7 @@
       <c r="N22" s="64"/>
       <c r="O22" s="64"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" s="64"/>
       <c r="B23" s="64"/>
       <c r="C23" s="64"/>
@@ -10422,7 +10450,7 @@
       <c r="N23" s="64"/>
       <c r="O23" s="64"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" s="64"/>
       <c r="B24" s="64"/>
       <c r="C24" s="64"/>
@@ -10439,7 +10467,7 @@
       <c r="N24" s="64"/>
       <c r="O24" s="64"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" s="64"/>
       <c r="B25" s="64"/>
       <c r="C25" s="64"/>
@@ -10456,7 +10484,7 @@
       <c r="N25" s="64"/>
       <c r="O25" s="64"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" s="64"/>
       <c r="B26" s="64"/>
       <c r="C26" s="64"/>
@@ -10473,7 +10501,7 @@
       <c r="N26" s="64"/>
       <c r="O26" s="64"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" s="64"/>
       <c r="B27" s="64"/>
       <c r="C27" s="64"/>
@@ -10490,7 +10518,7 @@
       <c r="N27" s="64"/>
       <c r="O27" s="64"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" s="64"/>
       <c r="B28" s="64"/>
       <c r="C28" s="64"/>
@@ -10507,7 +10535,7 @@
       <c r="N28" s="64"/>
       <c r="O28" s="64"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29" s="64"/>
       <c r="B29" s="64"/>
       <c r="C29" s="64"/>
@@ -10542,14 +10570,14 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="15.54296875" customWidth="1"/>
-    <col min="3" max="3" width="65.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.53515625" customWidth="1"/>
+    <col min="3" max="3" width="65.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="123" t="s">
         <v>3</v>
       </c>
@@ -10557,7 +10585,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B3" s="119" t="s">
         <v>331</v>
       </c>
@@ -10565,7 +10593,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B4" s="119" t="s">
         <v>330</v>
       </c>
@@ -10573,7 +10601,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B5" s="119" t="s">
         <v>330</v>
       </c>
@@ -10581,7 +10609,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B6" s="119" t="s">
         <v>334</v>
       </c>
@@ -10589,7 +10617,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B7" s="119" t="s">
         <v>330</v>
       </c>
@@ -10597,7 +10625,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B8" s="119" t="s">
         <v>330</v>
       </c>
@@ -10605,7 +10633,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B9" s="119" t="s">
         <v>330</v>
       </c>
@@ -10613,7 +10641,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B10" s="119" t="s">
         <v>360</v>
       </c>
@@ -10621,87 +10649,87 @@
         <v>361</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B11" s="119"/>
       <c r="C11" s="120"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B12" s="119"/>
       <c r="C12" s="120"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B13" s="119"/>
       <c r="C13" s="120"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B14" s="119"/>
       <c r="C14" s="120"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B15" s="119"/>
       <c r="C15" s="120"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B16" s="119"/>
       <c r="C16" s="120"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B17" s="119"/>
       <c r="C17" s="120"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B18" s="119"/>
       <c r="C18" s="120"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B19" s="119"/>
       <c r="C19" s="120"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B20" s="119"/>
       <c r="C20" s="120"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B21" s="119"/>
       <c r="C21" s="120"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B22" s="119"/>
       <c r="C22" s="120"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B23" s="119"/>
       <c r="C23" s="120"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B24" s="119"/>
       <c r="C24" s="120"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B25" s="119"/>
       <c r="C25" s="120"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B26" s="119"/>
       <c r="C26" s="120"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B27" s="119"/>
       <c r="C27" s="120"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B28" s="119"/>
       <c r="C28" s="120"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B29" s="119"/>
       <c r="C29" s="120"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B30" s="119"/>
       <c r="C30" s="120"/>
     </row>
-    <row r="31" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B31" s="121"/>
       <c r="C31" s="122"/>
     </row>

</xml_diff>